<commit_message>
Ajout des tâches du jour
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>Fonction permettant d'ajouter un article dans la base de données est fonctionnelle. Elle permet d'ajouter trois images, la marque et le modèle de l'article, la taille, la quantité et la couleur.</t>
+  </si>
+  <si>
+    <t>J'ai remarqué que quand j'ajoutai un article avec la même marque et le même modèle il y avait des soucis. Quand je mettais une chaussure jaune et qu'ensuite j'ajoutais la même en noir avec des tailles différentes, il y avait un problème lorsque je les ajoutais un de ces articles dans mon panier, dans certains cas ce n'était pas le bon que j'avais sélectionné. Du coup j'ai dû changer mes requête que je faisais à ma base de données pour avoir le bon article dans mon panier.</t>
+  </si>
+  <si>
+    <t>Documentation du projet, j'ai refait mon chapitre où je décris mon MLD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6ème semaine </t>
   </si>
 </sst>
 </file>
@@ -480,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,8 +867,38 @@
         <v>13</v>
       </c>
     </row>
+    <row r="39" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>43168</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>43168</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A41:C41"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A20:C20"/>

</xml_diff>

<commit_message>
Ajout des tâches du matin
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t xml:space="preserve">6ème semaine </t>
+  </si>
+  <si>
+    <t>Dans le coin en haut à droite de ma page il y a une petite icône qui sert à afficher le panier, j'ai fait en sorte que la petite fenêtre qui s'affiche quand on clique sur l'icône affiche ce qu'il y a dans le panier de l'utilisateur connecté. J'ai eu quelques soucis quand j'ai fait le developpement, j'ai dû mettre en forme ma page HTML pour que tout passe dans la petite fenêtre.</t>
+  </si>
+  <si>
+    <t>J'ai commencé à m'informer sur l'utilisation de ionic, je l'ai déjà installé sur mon poste pour pouvoir l'utiliser plus tard</t>
   </si>
 </sst>
 </file>
@@ -203,10 +209,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -489,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,11 +508,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -578,11 +584,11 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -671,11 +677,11 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
@@ -722,11 +728,11 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
@@ -806,11 +812,11 @@
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -890,11 +896,33 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>43172</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>43172</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Ajout d'une nouvelle tâche
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>J'ai commencé à m'informer sur l'utilisation de ionic, je l'ai déjà installé sur mon poste pour pouvoir l'utiliser plus tard</t>
+  </si>
+  <si>
+    <t>Je vais commencer par suivre ce tuto : https://www.youtube.com/watch?v=yWOAkwM3B9Y que j'ai trouvé sur youtube.</t>
   </si>
 </sst>
 </file>
@@ -495,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -922,6 +925,14 @@
       </c>
       <c r="C43" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43172</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout de l'activité d'aujourd'hui
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>J'ai commencé à faire des pages de tests avec ionic mais j'ai un problème quand je veux utiliser du jQuery, ça ne fonctionne pas. Je n'ai réussi à trouver la solution pour le faire fonctionner en utilisant jQuery.</t>
+  </si>
+  <si>
+    <t>J'ai créé un dossier qui contiendra mon application pour le téléphone sur le site de Ionic directement. Ce qui me permettra de faire mon développement sur l'ordinateur et de voir sur mon natel mon application. J'ai regardé avec M. Carrel avec quoi je devais démarrer et je dois commencer à implémenter la lecture des QR Code.</t>
   </si>
 </sst>
 </file>
@@ -501,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -950,6 +953,17 @@
       </c>
       <c r="C45" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>43174</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout des tâches de la journée
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -171,6 +171,18 @@
   </si>
   <si>
     <t>J'ai créé un dossier qui contiendra mon application pour le téléphone sur le site de Ionic directement. Ce qui me permettra de faire mon développement sur l'ordinateur et de voir sur mon natel mon application. J'ai regardé avec M. Carrel avec quoi je devais démarrer et je dois commencer à implémenter la lecture des QR Code.</t>
+  </si>
+  <si>
+    <t>J'ai commencé à implémenter mon QR Code avec l'aide de mon natel pour faire les tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7ème semaine </t>
+  </si>
+  <si>
+    <t>J'ai rempli ma documentation. J'ai fini la partie où je décris mes tables dans mon MLD</t>
+  </si>
+  <si>
+    <t>J'ai trouvé un tutoriel, pour scanner les qr code, que j'ai suivi sur youtube à cette adresse : https://www.youtube.com/watch?v=aa0abyOBa28. J'ai fait le tuto et je l'ai testé sur mon natel et ça fonctionne il me ressort des infos du qr code que je scanne. J'ai fini ma fonction qui me permet de recevoir la quantité d'article que j'ai dans ma base de données en scannant le QR Code avec l'id d'un article.</t>
   </si>
 </sst>
 </file>
@@ -504,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,8 +978,52 @@
         <v>13</v>
       </c>
     </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>43175</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+    </row>
+    <row r="49" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>43179</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C49" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>43179</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C50" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A48:C48"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A9:C9"/>

</xml_diff>

<commit_message>
Ajout des données dans la doc et journal de travail
Ajouter ce que j'ai aujourd'hui dans le journal de travail. J'ai ajouté et supprimé des choses dans la documentation du projet.
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -186,6 +186,12 @@
   </si>
   <si>
     <t xml:space="preserve">Dans mon application pour le mobile j'ai rajouté des valeurs comme une illustration de l'article, la marque, le modèle, etc. Ensuite lors de l'inscription sur les smartphones il y avait une erreur que j'ai réglé, je m'étais une valeure dans la session qui n'éxistait pas encore </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai fait une fonction pour le panier qui me permet d'afficher le nombre d'article présent dans le panier. Mais elle ne fonctionne pas à 100%, une fois que j'ajoute ou supprime un article dans mon panier, je dois recharger une nouvelle fois la page pour que ma fonction affiche le bon nombre. </t>
+  </si>
+  <si>
+    <t>J'ai ajouté des choses dans ma documentation de projet, comme mon nom par exemple que je n'avais pas mis. J'ai supprimé aussi des chapitres inutiles. J'ai aussi changé des choses dans certains chapitres et modifié la planification pour afficher seulement les activités.</t>
   </si>
 </sst>
 </file>
@@ -519,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1031,6 +1037,31 @@
       <c r="C51" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="52" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>43181</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C52" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>43182</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Ajout des activité de la journée
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -192,6 +192,15 @@
   </si>
   <si>
     <t>J'ai ajouté des choses dans ma documentation de projet, comme mon nom par exemple que je n'avais pas mis. J'ai supprimé aussi des chapitres inutiles. J'ai aussi changé des choses dans certains chapitres et modifié la planification pour afficher seulement les activités.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai eu un problème quand j'ajoutais un article dans un panier d'un utilisateur fraîchement créé. Mon article ne s'ajoutait pas la première fois que j'appuyais sur le bouton mais la deuxième fois. J'avais ajouté un un champ en trop dans ma requête qui faisait que ça ne fonctionnait pas. </t>
+  </si>
+  <si>
+    <t>J'ai aussi ajouté des contrôles lors de la connexion et de l'inscription, lorsque le mot de passe et faux à la connexion un message apparait. A l'inscription si le login est déjà utilisé par quelqu'un d'autre un message apparait.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M. Carrel est venu m'aider parce que j'avais un problème avec mon panier. Lorsque j'ajoutais et supprimait un article dans le panier d'un utilisateur, je devais rafraichir à nouveau la page pour que dans l'icône en haut à droite de ma page s'affiche mes articles dans le panier et le nombre que j'ai d'article dedans. J'ai changé de place un require_once pour que mon affichage de mon menu se fassent après le traitement des données. </t>
   </si>
 </sst>
 </file>
@@ -525,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1061,10 +1070,48 @@
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
+      <c r="A54" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" s="3"/>
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>43186</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>43186</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C56" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>43186</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" t="s">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="A54:C54"/>
     <mergeCell ref="A48:C48"/>
     <mergeCell ref="A41:C41"/>
     <mergeCell ref="A1:C1"/>

</xml_diff>

<commit_message>
Ajout de l'activité de la journée
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\Pre-TPi\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/Pre-TPi/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B4FD8CED-2428-BA43-935E-32D6CDE3C760}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -201,12 +202,15 @@
   </si>
   <si>
     <t xml:space="preserve">M. Carrel est venu m'aider parce que j'avais un problème avec mon panier. Lorsque j'ajoutais et supprimait un article dans le panier d'un utilisateur, je devais rafraichir à nouveau la page pour que dans l'icône en haut à droite de ma page s'affiche mes articles dans le panier et le nombre que j'ai d'article dedans. J'ai changé de place un require_once pour que mon affichage de mon menu se fassent après le traitement des données. </t>
+  </si>
+  <si>
+    <t>J'ai géré la partie des quantités dans mon panier et dans la base de données. Quand j'ajoute un article dans le panier il soustrait un dans la BD. Quand je supprime un article dans le panier il ajoute la quantité que j'ai dans mon panier dans la BD. J'ai aussi amélioré le total des prix dans le panier, il va d'abord multiplier le nombre de fois que j'ai le même article dans le panier et tout additionner ensemble.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -533,27 +537,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="82.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="82.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43132</v>
       </c>
@@ -564,7 +568,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43132</v>
       </c>
@@ -575,7 +579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43132</v>
       </c>
@@ -586,10 +590,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43133</v>
       </c>
@@ -600,7 +604,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43133</v>
       </c>
@@ -611,7 +615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43133</v>
       </c>
@@ -622,14 +626,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>43137</v>
       </c>
@@ -640,7 +644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>43137</v>
       </c>
@@ -651,10 +655,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>43138</v>
       </c>
@@ -665,10 +669,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>43139</v>
       </c>
@@ -679,10 +683,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>43140</v>
       </c>
@@ -693,7 +697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>43140</v>
       </c>
@@ -704,7 +708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>43140</v>
       </c>
@@ -715,14 +719,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
     </row>
-    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>43144</v>
       </c>
@@ -733,7 +737,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>43145</v>
       </c>
@@ -744,7 +748,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>43146</v>
       </c>
@@ -755,7 +759,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>43147</v>
       </c>
@@ -766,14 +770,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
     </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>42793</v>
       </c>
@@ -784,7 +788,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>43158</v>
       </c>
@@ -795,7 +799,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>43159</v>
       </c>
@@ -806,7 +810,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43160</v>
       </c>
@@ -817,7 +821,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43160</v>
       </c>
@@ -828,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>42796</v>
       </c>
@@ -839,7 +843,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43161</v>
       </c>
@@ -850,14 +854,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43165</v>
       </c>
@@ -868,7 +872,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43165</v>
       </c>
@@ -879,7 +883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43165</v>
       </c>
@@ -890,7 +894,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43166</v>
       </c>
@@ -901,7 +905,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43167</v>
       </c>
@@ -912,7 +916,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43168</v>
       </c>
@@ -923,7 +927,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43168</v>
       </c>
@@ -934,14 +938,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
     </row>
-    <row r="42" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43172</v>
       </c>
@@ -952,7 +956,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43172</v>
       </c>
@@ -963,7 +967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43172</v>
       </c>
@@ -974,7 +978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43173</v>
       </c>
@@ -985,7 +989,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43174</v>
       </c>
@@ -996,7 +1000,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43175</v>
       </c>
@@ -1007,14 +1011,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
     </row>
-    <row r="49" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>43179</v>
       </c>
@@ -1025,7 +1029,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>43179</v>
       </c>
@@ -1036,7 +1040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>43180</v>
       </c>
@@ -1047,7 +1051,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>43181</v>
       </c>
@@ -1058,7 +1062,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>43182</v>
       </c>
@@ -1069,14 +1073,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
     </row>
-    <row r="55" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>43186</v>
       </c>
@@ -1084,10 +1088,10 @@
         <v>55</v>
       </c>
       <c r="C55" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>43186</v>
       </c>
@@ -1095,10 +1099,10 @@
         <v>56</v>
       </c>
       <c r="C56" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="75" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>43186</v>
       </c>
@@ -1107,6 +1111,17 @@
       </c>
       <c r="C57" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="60" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
+        <v>43186</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout des activités de la journée
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10319"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10410"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/Pre-TPi/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{DCEDAF74-CADD-8140-994D-5342B59E73C9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7A4DDED7-47AE-A94A-A0E8-000606D5E528}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="64">
   <si>
     <t>Début du projet, lire le cahier des charges du projet</t>
   </si>
@@ -211,6 +211,15 @@
   </si>
   <si>
     <t>Ajout de différentes informations sur la page d'acceuil du site, j'ai ajouté les trois catégories que je propose sur le site comme ça les gens n'ont plus qu'à cliquer sur la catégorie qui les intéresse et seront dirgié vers celle-ci. Ensuite en bas de page j'ai affiché une dizaine d'article que je récupère aléatoirement dans la base de données. Les gens clique sur le bouton et sont dirigés vers l'article pour le commander.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8ème semaine </t>
+  </si>
+  <si>
+    <t>J'ai changé le nom de ma base de données, j'ai géré les injections sql pour le site.</t>
+  </si>
+  <si>
+    <t>J'ai rempli ma documentation, j'ai fait ma conclusion et j'ai ajouté des choses dans mon tableau de bord. J'ai ajouté aussi des choses dans le journal de bord.</t>
   </si>
 </sst>
 </file>
@@ -544,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C60"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="143" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1152,8 +1161,38 @@
         <v>13</v>
       </c>
     </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>43207</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>43207</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C63" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A61:C61"/>
     <mergeCell ref="A54:C54"/>
     <mergeCell ref="A48:C48"/>
     <mergeCell ref="A41:C41"/>

</xml_diff>

<commit_message>
Ajout de l'activité de l'après-midi
</commit_message>
<xml_diff>
--- a/Documentation/Journal_de_travail.xlsx
+++ b/Documentation/Journal_de_travail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/Pre-TPi/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7A4DDED7-47AE-A94A-A0E8-000606D5E528}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{03079255-3990-7C43-B4A2-1707080F3EAA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1176,7 +1176,7 @@
         <v>63</v>
       </c>
       <c r="C62" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>